<commit_message>
fazendo as análises de comparação
</commit_message>
<xml_diff>
--- a/mythril/teste_0.24.7_smartbugs-curated/teste_0.24.7_mythril_smartbugs-curatedresult_dasp.xlsx
+++ b/mythril/teste_0.24.7_smartbugs-curated/teste_0.24.7_mythril_smartbugs-curatedresult_dasp.xlsx
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>2</v>

</xml_diff>